<commit_message>
giant_se and http local server
</commit_message>
<xml_diff>
--- a/giant_se/rsc/TABLE정보.xlsx
+++ b/giant_se/rsc/TABLE정보.xlsx
@@ -400,56 +400,58 @@
   </si>
   <si>
     <t>ftk_uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(128)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url_img</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url_uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>store</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmp_uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>factory_key_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ftk_uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>url</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(128)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>url_img</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>URL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>url_uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>store</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cmp_uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(20)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>factory_key_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -880,11 +882,11 @@
   <dimension ref="B2:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="2" x14ac:dyDescent="0.3"/>
@@ -1264,7 +1266,7 @@
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
       <c r="C25" s="3" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>4</v>
@@ -1292,7 +1294,7 @@
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="10"/>
       <c r="C27" s="3" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>27</v>
@@ -1306,10 +1308,10 @@
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="10"/>
       <c r="C28" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>14</v>
@@ -1320,10 +1322,10 @@
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="10"/>
       <c r="C29" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>14</v>
@@ -1400,7 +1402,7 @@
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="10"/>
       <c r="C34" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>4</v>
@@ -1418,7 +1420,7 @@
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="10"/>
       <c r="C35" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>96</v>
@@ -1493,7 +1495,7 @@
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>1</v>
@@ -1514,7 +1516,7 @@
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="10"/>
       <c r="C41" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>4</v>
@@ -1532,10 +1534,10 @@
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
       <c r="C42" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>13</v>
@@ -1548,7 +1550,7 @@
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" s="10"/>
       <c r="C43" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>27</v>
@@ -1562,7 +1564,7 @@
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="10"/>
       <c r="C44" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>27</v>
@@ -1576,7 +1578,7 @@
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" s="10"/>
       <c r="C45" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>81</v>

</xml_diff>